<commit_message>
Adapted MC_industry file to reduced input, adapted RECC_Config to read ind and app products
</commit_message>
<xml_diff>
--- a/MESSAGE/Copper_MI.xlsx
+++ b/MESSAGE/Copper_MI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklose\Documents\ODYM-RECC-Repos\ODYM-RECC-Repo\RECC-ODYM\IAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklose\Documents\ODYM-RECC-Repos\RECC-Cu-Repo\ODYM-RECC Cu\MESSAGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>IGCC power plant with CCS</t>
-  </si>
-  <si>
     <t>solar photovoltaic power plant</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Copper content [kt/GW]</t>
+  </si>
+  <si>
+    <t>coal power plant with CCS</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -407,146 +407,133 @@
     <col min="6" max="6" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>6.3420000000000005</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>3.1459999999999999</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>2.7305000000000001</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>5.5715000000000003</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>1.6990000000000001</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0.76500000000000001</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>1.1460000000000001</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>0.76200000000000001</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>0.76200000000000001</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0.5</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>1.0515000000000001</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>6.2830000000000004</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1.6300000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>3.6295000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>5.5149999999999997</v>
       </c>
-      <c r="F16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>